<commit_message>
Fixed small mistake on the ideal burndown formula
</commit_message>
<xml_diff>
--- a/Project/Phase 2/Sprint 1/Burndown chart.xlsx
+++ b/Project/Phase 2/Sprint 1/Burndown chart.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Arruda\Desktop\Phase 2\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D886F41-F2B3-42C3-B0B7-2A2AAD411EBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burndown Chart" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -23,6 +24,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -77,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="[$-409]d/mmm/yy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -588,7 +591,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="pt-PT"/>
   <c:roundedCorners val="0"/>
@@ -627,7 +630,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -709,7 +711,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-8D0E-4F8E-897D-5B1720B3868B}"/>
             </c:ext>
@@ -811,7 +813,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-8D0E-4F8E-897D-5B1720B3868B}"/>
             </c:ext>
@@ -873,19 +875,19 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.666666666666667</c:v>
+                  <c:v>3.333333333333333</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.333333333333333</c:v>
+                  <c:v>1.6666666666666665</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-8D0E-4F8E-897D-5B1720B3868B}"/>
             </c:ext>
@@ -1004,7 +1006,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1079,7 +1080,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1111,14 +1111,14 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1729,7 +1729,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52BFCA64-3DDA-4711-BDFA-D2973C7C7C4B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2046,11 +2046,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2260,16 +2260,16 @@
         <v>5</v>
       </c>
       <c r="E13" s="18">
-        <f>$D$13-($D$13/15*1)</f>
-        <v>4.666666666666667</v>
+        <f>$D$13-($D$13/3*1)</f>
+        <v>3.333333333333333</v>
       </c>
       <c r="F13" s="1">
-        <f>$D$13-($D$13/15*2)</f>
-        <v>4.333333333333333</v>
+        <f>$D$13-($D$13/3*2)</f>
+        <v>1.6666666666666665</v>
       </c>
       <c r="G13" s="1">
-        <f>$D$13-($D$13/15*3)</f>
-        <v>4</v>
+        <f>$D$13-($D$13/3*3)</f>
+        <v>0</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>

</xml_diff>